<commit_message>
Add Arlequin Fs runs
</commit_message>
<xml_diff>
--- a/popgen_stats/Dongsha_stats.xlsx
+++ b/popgen_stats/Dongsha_stats.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eric/github/dongsha/popgen_stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5246951-2766-B44C-9AC0-95FAC417C45F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656AC9CB-643C-A84F-8C0D-DE46D1C33E14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25160" yWindow="3660" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19160" yWindow="7500" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dongsha_stats" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1087,14 +1086,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:A27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" customWidth="1"/>
+    <col min="8" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1643,13 +1644,13 @@
         <v>-10.079151814247099</v>
       </c>
       <c r="P10">
-        <v>-26.7161422629468</v>
+        <v>-8.8129660469340791</v>
       </c>
       <c r="Q10">
-        <v>63.778515416737399</v>
+        <v>2.2255096914532699</v>
       </c>
       <c r="R10">
-        <v>0.76921693411803804</v>
+        <v>9.3762768387526799E-2</v>
       </c>
       <c r="S10">
         <v>0.36200834536162702</v>
@@ -2034,7 +2035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72349590-5B79-B74C-9457-2822CF3EC1F7}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>

</xml_diff>